<commit_message>
Filled out the rest of the asset list. Only thing left is sound.
</commit_message>
<xml_diff>
--- a/Docs/Design/AssetList.xlsx
+++ b/Docs/Design/AssetList.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="13395" windowHeight="7740"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="13395" windowHeight="7740" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Animations" sheetId="1" r:id="rId1"/>
+    <sheet name="Level Backgrounds" sheetId="2" r:id="rId2"/>
+    <sheet name="Sound" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="37">
   <si>
     <t>Creature</t>
   </si>
@@ -61,6 +61,72 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Spy</t>
+  </si>
+  <si>
+    <t>Trojan</t>
+  </si>
+  <si>
+    <t>Special</t>
+  </si>
+  <si>
+    <t>Addy</t>
+  </si>
+  <si>
+    <t>Copy Cat</t>
+  </si>
+  <si>
+    <t>Roid</t>
+  </si>
+  <si>
+    <t>Root Kit</t>
+  </si>
+  <si>
+    <t>Ghost</t>
+  </si>
+  <si>
+    <t>Infestation Swarm</t>
+  </si>
+  <si>
+    <t>TNT</t>
+  </si>
+  <si>
+    <t>System Link</t>
+  </si>
+  <si>
+    <t>Zero</t>
+  </si>
+  <si>
+    <t>Muncher</t>
+  </si>
+  <si>
+    <t>Spammer</t>
+  </si>
+  <si>
+    <t>Worm</t>
+  </si>
+  <si>
+    <t>Slicer</t>
+  </si>
+  <si>
+    <t>Freezer</t>
+  </si>
+  <si>
+    <t>Parasite</t>
+  </si>
+  <si>
+    <t>Re-Direct</t>
+  </si>
+  <si>
+    <t>Zdoc</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>To Do</t>
   </si>
 </sst>
 </file>
@@ -399,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +476,7 @@
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,8 +495,11 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -449,8 +518,11 @@
       <c r="F2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -469,8 +541,11 @@
       <c r="F3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -489,8 +564,11 @@
       <c r="F4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -509,8 +587,11 @@
       <c r="F5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -529,8 +610,11 @@
       <c r="F6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -548,6 +632,446 @@
       </c>
       <c r="F7" t="s">
         <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -557,12 +1081,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -571,10 +1128,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a few more assets to the list
</commit_message>
<xml_diff>
--- a/Docs/Design/AssetList.xlsx
+++ b/Docs/Design/AssetList.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="13395" windowHeight="7740" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="13395" windowHeight="7740"/>
   </bookViews>
   <sheets>
-    <sheet name="Animations" sheetId="1" r:id="rId1"/>
-    <sheet name="Level Backgrounds" sheetId="2" r:id="rId2"/>
+    <sheet name="Other Art" sheetId="4" r:id="rId1"/>
+    <sheet name="Animations" sheetId="1" r:id="rId2"/>
     <sheet name="Sound" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="43">
   <si>
     <t>Creature</t>
   </si>
@@ -123,16 +123,37 @@
     <t>Zdoc</t>
   </si>
   <si>
-    <t>Level</t>
-  </si>
-  <si>
     <t>To Do</t>
+  </si>
+  <si>
+    <t>Selector</t>
+  </si>
+  <si>
+    <t>Fog</t>
+  </si>
+  <si>
+    <t>Select Creature Screen</t>
+  </si>
+  <si>
+    <t>Main Menu Screen</t>
+  </si>
+  <si>
+    <t>Options Screen</t>
+  </si>
+  <si>
+    <t>Pause Menu</t>
+  </si>
+  <si>
+    <t>Level Backgrounds (5)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -162,8 +183,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,10 +487,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +551,7 @@
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +574,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -522,7 +597,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -544,8 +619,9 @@
       <c r="G3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -567,8 +643,9 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -591,7 +668,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -614,7 +691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -637,7 +714,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -660,7 +737,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -683,7 +760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -706,7 +783,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -729,7 +806,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -752,7 +829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -775,7 +852,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -798,7 +875,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -821,7 +898,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1072,51 +1149,6 @@
       </c>
       <c r="G26" t="s">
         <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1128,15 +1160,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>